<commit_message>
piccole modifiche e aggiunti set dati
Former-commit-id: f3fd16460bde1e9737a91104dbd8088ffd58ecbd [formerly ba071ceab179ca159ef547abc26055a4dfb9e107] [formerly 177f3051f550ceae58b802252bc8dc63b687bf7c [formerly 856f4da8f5af86907c249c7bc8bad91ca2d8861f]]
Former-commit-id: 1e08c4248c5cd0b5d72332a14bf3fb34e90d3b98 [formerly 0d1ec6af7a65617ce460a1f45e724fd19af388df]
Former-commit-id: f32f1022407fa1bd6052305de17484990b813497
</commit_message>
<xml_diff>
--- a/src/pyoma2/test_data/palisaden/geom.xlsx
+++ b/src/pyoma2/test_data/palisaden/geom.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://treteknisk-my.sharepoint.com/personal/dpa_treteknisk_no/Documents/Dokumenter/GITHUB REPO/pyOMA2/pyOMA2/test_pyOMA/test_data/palisaden/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://treteknisk-my.sharepoint.com/personal/dpa_treteknisk_no/Documents/Dokumenter/Dev/pyOMA2/src/pyoma2/test_data/palisaden/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="8_{6F673B9C-602E-4DCD-95D0-A3C55099C5FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D5C872B5-B2FA-48BA-AB17-DDE8D5E5621E}"/>
+  <xr:revisionPtr revIDLastSave="51" documentId="8_{6F673B9C-602E-4DCD-95D0-A3C55099C5FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EFF52124-5082-4094-8986-BFD20CE8039A}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="5895" yWindow="4095" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BG_nodes" sheetId="1" r:id="rId1"/>
     <sheet name="BG_lines" sheetId="2" r:id="rId2"/>
     <sheet name="Geo1" sheetId="3" r:id="rId3"/>
     <sheet name="Geo2" sheetId="4" r:id="rId4"/>
-    <sheet name="PhiExp" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="14">
   <si>
     <t>x</t>
   </si>
@@ -78,10 +77,10 @@
     <t>sName</t>
   </si>
   <si>
-    <t>TEST</t>
-  </si>
-  <si>
-    <t>BG_name</t>
+    <t>start</t>
+  </si>
+  <si>
+    <t>end</t>
   </si>
 </sst>
 </file>
@@ -89,7 +88,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -136,7 +135,7 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -418,31 +417,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T13" sqref="T13"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -450,105 +446,81 @@
       <c r="C2">
         <v>0</v>
       </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>15</v>
       </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
       <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>15</v>
       </c>
-      <c r="C4">
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>15</v>
+      </c>
+      <c r="B8">
         <v>10</v>
       </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
+      <c r="C8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="B9">
         <v>10</v>
       </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>15</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>15</v>
-      </c>
-      <c r="C8">
-        <v>10</v>
-      </c>
-      <c r="D8">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
       <c r="C9">
-        <v>10</v>
-      </c>
-      <c r="D9">
         <v>20</v>
       </c>
     </row>
@@ -559,75 +531,83 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F711F53-50B1-4D99-8D31-73D3733672B9}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B8"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>1</v>
-      </c>
-      <c r="B1">
-        <v>5</v>
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
         <v>6</v>
-      </c>
-      <c r="B6">
-        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
         <v>7</v>
-      </c>
-      <c r="B7">
-        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
         <v>5</v>
       </c>
     </row>
@@ -638,10 +618,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DACC31A-B50A-4C70-9F83-8C110CD77A88}">
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:D16"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -650,17 +630,17 @@
       <c r="A1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="H1" t="s">
         <v>0</v>
@@ -676,18 +656,17 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2">
-        <v>2</v>
-      </c>
-      <c r="C2">
-        <f>10-2</f>
-        <v>8</v>
+      <c r="C2" t="s">
+        <v>7</v>
       </c>
       <c r="D2">
-        <v>20</v>
-      </c>
-      <c r="F2" t="s">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>20</v>
       </c>
       <c r="H2">
         <v>-1</v>
@@ -704,18 +683,17 @@
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <f>10-2</f>
+      <c r="C3" t="s">
         <v>8</v>
       </c>
       <c r="D3">
-        <v>20</v>
-      </c>
-      <c r="F3" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>20</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -732,18 +710,18 @@
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4">
-        <f>15-4</f>
-        <v>11</v>
-      </c>
-      <c r="C4">
-        <v>8</v>
+      <c r="C4" t="s">
+        <v>3</v>
       </c>
       <c r="D4">
-        <v>20</v>
-      </c>
-      <c r="F4" t="s">
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <f>10-2</f>
+        <v>8</v>
+      </c>
+      <c r="F4">
+        <v>20</v>
       </c>
       <c r="H4">
         <v>-1</v>
@@ -760,18 +738,18 @@
       <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B5">
-        <f>15-4</f>
-        <v>11</v>
-      </c>
-      <c r="C5">
-        <v>8</v>
+      <c r="C5" t="s">
+        <v>4</v>
       </c>
       <c r="D5">
-        <v>20</v>
-      </c>
-      <c r="F5" t="s">
-        <v>6</v>
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <f>10-2</f>
+        <v>8</v>
+      </c>
+      <c r="F5">
+        <v>20</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -788,17 +766,18 @@
       <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-      <c r="C6">
-        <v>2</v>
+      <c r="C6" t="s">
+        <v>5</v>
       </c>
       <c r="D6">
-        <v>20</v>
-      </c>
-      <c r="F6" t="s">
-        <v>7</v>
+        <f>15-4</f>
+        <v>11</v>
+      </c>
+      <c r="E6">
+        <v>8</v>
+      </c>
+      <c r="F6">
+        <v>20</v>
       </c>
       <c r="H6">
         <v>-1</v>
@@ -815,135 +794,29 @@
       <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="B7">
-        <v>5</v>
-      </c>
-      <c r="C7">
-        <v>2</v>
+      <c r="C7" t="s">
+        <v>6</v>
       </c>
       <c r="D7">
-        <v>20</v>
-      </c>
-      <c r="F7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>1</v>
-      </c>
-      <c r="J7" s="2">
-        <v>0</v>
-      </c>
-      <c r="L7" s="1"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11">
-        <v>5</v>
-      </c>
-      <c r="C11">
-        <v>2</v>
-      </c>
-      <c r="D11">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12">
-        <v>5</v>
-      </c>
-      <c r="C12">
-        <v>2</v>
-      </c>
-      <c r="D12">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13">
-        <v>2</v>
-      </c>
-      <c r="C13">
-        <f>10-2</f>
-        <v>8</v>
-      </c>
-      <c r="D13">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14">
-        <v>2</v>
-      </c>
-      <c r="C14">
-        <f>10-2</f>
-        <v>8</v>
-      </c>
-      <c r="D14">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15">
         <f>15-4</f>
         <v>11</v>
       </c>
-      <c r="C15">
-        <v>8</v>
-      </c>
-      <c r="D15">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16">
-        <f>15-4</f>
-        <v>11</v>
-      </c>
-      <c r="C16">
-        <v>8</v>
-      </c>
-      <c r="D16">
-        <v>20</v>
-      </c>
+      <c r="E7">
+        <v>8</v>
+      </c>
+      <c r="F7">
+        <v>20</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7" s="2">
+        <v>0</v>
+      </c>
+      <c r="L7" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -954,29 +827,29 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D1D5F43-55C8-4FDF-B1E5-7D3B04642CE2}">
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E9"/>
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="H1" t="s">
         <v>9</v>
@@ -996,23 +869,28 @@
       <c r="N1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>2</v>
+      <c r="P1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
       </c>
       <c r="C2">
-        <f>10-2</f>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <v>20</v>
-      </c>
-      <c r="F2" t="s">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>8</v>
+      </c>
+      <c r="F2">
+        <v>20</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -1032,23 +910,28 @@
       <c r="N2">
         <v>-1</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <f>15-4</f>
+      <c r="P2">
+        <v>4</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
         <v>11</v>
       </c>
-      <c r="C3">
-        <v>8</v>
-      </c>
-      <c r="D3">
-        <v>20</v>
-      </c>
-      <c r="F3" t="s">
-        <v>4</v>
+      <c r="E3">
+        <v>8</v>
+      </c>
+      <c r="F3">
+        <v>20</v>
       </c>
       <c r="H3">
         <v>2</v>
@@ -1068,22 +951,28 @@
       <c r="N3">
         <v>-1</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="P3">
+        <v>5</v>
+      </c>
+      <c r="Q3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>5</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
       <c r="D4">
-        <v>20</v>
-      </c>
-      <c r="F4" t="s">
-        <v>5</v>
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>20</v>
       </c>
       <c r="H4">
         <v>3</v>
@@ -1103,57 +992,69 @@
       <c r="N4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="P4">
+        <v>6</v>
+      </c>
+      <c r="Q4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5">
         <v>4</v>
       </c>
-      <c r="B5">
-        <v>11</v>
-      </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
       <c r="D5">
-        <v>20</v>
-      </c>
-      <c r="F5" t="s">
-        <v>6</v>
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>8</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
       </c>
       <c r="H5">
         <v>4</v>
       </c>
-      <c r="I5" t="s">
-        <v>7</v>
-      </c>
-      <c r="J5" t="s">
-        <v>6</v>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
       </c>
       <c r="L5">
         <v>4</v>
       </c>
       <c r="M5">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="N5">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
+      <c r="Q5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
       </c>
       <c r="C6">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="F6" t="s">
-        <v>7</v>
+        <v>11</v>
+      </c>
+      <c r="E6">
+        <v>8</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
       </c>
       <c r="H6">
         <v>5</v>
@@ -1173,22 +1074,28 @@
       <c r="N6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="P6">
+        <v>2</v>
+      </c>
+      <c r="Q6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7">
         <v>6</v>
       </c>
-      <c r="B7">
-        <v>11</v>
-      </c>
-      <c r="C7">
-        <v>8</v>
-      </c>
       <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="F7" t="s">
-        <v>8</v>
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
       </c>
       <c r="H7">
         <v>6</v>
@@ -1208,150 +1115,11 @@
       <c r="N7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>5</v>
-      </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>7</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="L8">
-        <v>7</v>
-      </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
-      <c r="N8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>11</v>
-      </c>
-      <c r="C9">
-        <v>2</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>8</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
-      <c r="L9">
-        <v>8</v>
-      </c>
-      <c r="M9">
-        <v>0</v>
-      </c>
-      <c r="N9">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C72FE6C5-F577-42EB-8BCA-A588E0831C8B}">
-  <dimension ref="A1:C6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1">
-        <v>1.42157E-2</v>
-      </c>
-      <c r="B1" s="1">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1">
-        <v>0.50000599999999995</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>0.85671299999999995</v>
-      </c>
-      <c r="B2" s="1">
-        <v>0.18603800000000001</v>
-      </c>
-      <c r="C2" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>9.4731200000000002E-2</v>
-      </c>
-      <c r="B3" s="1">
-        <v>0.98106400000000005</v>
-      </c>
-      <c r="C3" s="1">
-        <v>0.36526399999999998</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>1</v>
-      </c>
-      <c r="B4" s="1">
-        <v>-6.8085999999999994E-2</v>
-      </c>
-      <c r="C4" s="1">
-        <v>-0.62785199999999997</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>3.2213600000000002E-2</v>
-      </c>
-      <c r="B5" s="1">
-        <v>0.86719199999999996</v>
-      </c>
-      <c r="C5" s="1">
-        <v>-0.58319799999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>-0.88529800000000003</v>
-      </c>
-      <c r="B6" s="1">
-        <v>-9.6825999999999995E-2</v>
-      </c>
-      <c r="C6" s="1">
-        <v>-0.69423100000000004</v>
+      <c r="P7">
+        <v>3</v>
+      </c>
+      <c r="Q7">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>